<commit_message>
Running a test with numpy arrays and NaN values.
</commit_message>
<xml_diff>
--- a/database/AN_ep/expdata/1003.xlsx
+++ b/database/AN_ep/expdata/1003.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malda\Documents\GitHub\jam3d\database\AN_ep\expdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06701E90-AD1A-4C12-A00D-E54003676475}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721FCA6D-1515-4CB1-AB87-C3D0FA68FFD9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16890" yWindow="1422" windowWidth="9870" windowHeight="8172" xr2:uid="{D5643214-696F-4D74-AD1B-BB38719F35C1}"/>
+    <workbookView xWindow="2736" yWindow="2268" windowWidth="9870" windowHeight="8172" xr2:uid="{D5643214-696F-4D74-AD1B-BB38719F35C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -426,8 +426,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94CFD0E6-D78E-48DF-BC57-D3E7799F4DAC}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -472,13 +472,13 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F2">
         <v>63</v>
@@ -504,13 +504,13 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E3">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F3">
         <v>63</v>
@@ -536,13 +536,13 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="D4">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E4">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F4">
         <v>63</v>
@@ -568,13 +568,13 @@
         <v>3</v>
       </c>
       <c r="C5">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="D5">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E5">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F5">
         <v>63</v>
@@ -600,13 +600,13 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="D6">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F6">
         <v>63</v>
@@ -632,13 +632,13 @@
         <v>3</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E7">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F7">
         <v>63</v>
@@ -664,13 +664,13 @@
         <v>3</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E8">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F8">
         <v>63</v>
@@ -696,13 +696,13 @@
         <v>3</v>
       </c>
       <c r="C9">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="D9">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E9">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F9">
         <v>63</v>
@@ -728,13 +728,13 @@
         <v>3</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E10">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F10">
         <v>63</v>
@@ -760,13 +760,13 @@
         <v>3</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="D11">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F11">
         <v>63</v>
@@ -792,13 +792,13 @@
         <v>3</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F12">
         <v>63</v>
@@ -824,13 +824,13 @@
         <v>3</v>
       </c>
       <c r="C13">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="D13">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F13">
         <v>63</v>
@@ -856,13 +856,13 @@
         <v>3</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="D14">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F14">
         <v>63</v>
@@ -888,13 +888,13 @@
         <v>3</v>
       </c>
       <c r="C15">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F15">
         <v>63</v>
@@ -920,13 +920,13 @@
         <v>3</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E16">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F16">
         <v>63</v>
@@ -952,13 +952,13 @@
         <v>3</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="D17">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E17">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F17">
         <v>63</v>
@@ -984,13 +984,13 @@
         <v>3</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="D18">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="E18">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="F18">
         <v>63</v>

</xml_diff>

<commit_message>
Updated data files with integers as floats.
</commit_message>
<xml_diff>
--- a/database/AN_ep/expdata/1003.xlsx
+++ b/database/AN_ep/expdata/1003.xlsx
@@ -138,7 +138,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -148,10 +148,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -175,7 +171,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
+      <selection pane="topLeft" activeCell="D22" activeCellId="0" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -469,8 +465,8 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="n">
-        <v>0.001</v>
+      <c r="A10" s="2" t="n">
+        <v>0</v>
       </c>
       <c r="B10" s="2" t="n">
         <v>3</v>

</xml_diff>

<commit_message>
Fixed data sheets back to root s of 63 GeV
</commit_message>
<xml_diff>
--- a/database/AN_ep/expdata/1003.xlsx
+++ b/database/AN_ep/expdata/1003.xlsx
@@ -225,7 +225,7 @@
         <v>0.001</v>
       </c>
       <c r="F2" s="2" t="n">
-        <v>125</v>
+        <v>63</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>10</v>
@@ -257,7 +257,7 @@
         <v>0.001</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>125</v>
+        <v>63</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>10</v>
@@ -289,7 +289,7 @@
         <v>0.001</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>125</v>
+        <v>63</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>10</v>
@@ -321,7 +321,7 @@
         <v>0.001</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>125</v>
+        <v>63</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>10</v>
@@ -353,7 +353,7 @@
         <v>0.001</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>125</v>
+        <v>63</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>10</v>
@@ -385,7 +385,7 @@
         <v>0.001</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>125</v>
+        <v>63</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>10</v>
@@ -417,7 +417,7 @@
         <v>0.001</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>125</v>
+        <v>63</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>10</v>
@@ -449,7 +449,7 @@
         <v>0.001</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>125</v>
+        <v>63</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>10</v>
@@ -481,7 +481,7 @@
         <v>0.001</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>125</v>
+        <v>63</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>10</v>
@@ -513,7 +513,7 @@
         <v>0.001</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>125</v>
+        <v>63</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>10</v>
@@ -545,7 +545,7 @@
         <v>0.001</v>
       </c>
       <c r="F12" s="2" t="n">
-        <v>125</v>
+        <v>63</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>10</v>
@@ -577,7 +577,7 @@
         <v>0.001</v>
       </c>
       <c r="F13" s="2" t="n">
-        <v>125</v>
+        <v>63</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>10</v>
@@ -609,7 +609,7 @@
         <v>0.001</v>
       </c>
       <c r="F14" s="2" t="n">
-        <v>125</v>
+        <v>63</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>10</v>
@@ -641,7 +641,7 @@
         <v>0.001</v>
       </c>
       <c r="F15" s="2" t="n">
-        <v>125</v>
+        <v>63</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>10</v>
@@ -673,7 +673,7 @@
         <v>0.001</v>
       </c>
       <c r="F16" s="2" t="n">
-        <v>125</v>
+        <v>63</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>10</v>
@@ -705,7 +705,7 @@
         <v>0.001</v>
       </c>
       <c r="F17" s="2" t="n">
-        <v>125</v>
+        <v>63</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>10</v>
@@ -737,7 +737,7 @@
         <v>0.001</v>
       </c>
       <c r="F18" s="2" t="n">
-        <v>125</v>
+        <v>63</v>
       </c>
       <c r="G18" s="1" t="s">
         <v>10</v>

</xml_diff>